<commit_message>
Major revamp (Digit, SudokuGrid, DigitSet) + SudokuGrader
</commit_message>
<xml_diff>
--- a/scratchpad/symmetry_indices.xlsx
+++ b/scratchpad/symmetry_indices.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/workbench/SudokuWizard/scratchpad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85CC0313-6A0A-D146-A731-A93A869DFE0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E0515D-EF50-C740-9834-0D4EF7B5A940}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19240" yWindow="4560" windowWidth="23960" windowHeight="17440" xr2:uid="{07FB0925-E1A7-7E43-9070-809CA48C8E41}"/>
+    <workbookView xWindow="29400" yWindow="460" windowWidth="13220" windowHeight="17360" activeTab="1" xr2:uid="{07FB0925-E1A7-7E43-9070-809CA48C8E41}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="symmetry" sheetId="1" r:id="rId1"/>
+    <sheet name="hidden singles" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>r = i/9</t>
   </si>
@@ -50,12 +51,72 @@
   <si>
     <t>I' = 9*(i%9) + 8 - i/9</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>~B</t>
+  </si>
+  <si>
+    <t>A ^ ~B</t>
+  </si>
+  <si>
+    <t>~A</t>
+  </si>
+  <si>
+    <t>~A v B</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>a+b - a*b</t>
+  </si>
+  <si>
+    <t>a*b</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>1-a</t>
+  </si>
+  <si>
+    <t>~A v B1</t>
+  </si>
+  <si>
+    <t>v B2</t>
+  </si>
+  <si>
+    <t>v B3</t>
+  </si>
+  <si>
+    <t>v B4</t>
+  </si>
+  <si>
+    <t>v B5</t>
+  </si>
+  <si>
+    <t>v B6</t>
+  </si>
+  <si>
+    <t>v B7</t>
+  </si>
+  <si>
+    <t>v B8</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -66,6 +127,14 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -205,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,6 +328,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -577,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867BB34E-53AF-D142-89A8-873DB405F165}">
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -601,7 +673,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="3">
-        <f t="shared" ref="D1:D21" si="0">80-C1</f>
+        <f t="shared" ref="D1:D20" si="0">80-C1</f>
         <v>72</v>
       </c>
       <c r="G1" s="15">
@@ -2443,4 +2515,1140 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DF1539-E103-F04B-9E2A-1C0C3B8DBAE0}">
+  <dimension ref="B1:M32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="10" width="4.1640625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B1" s="19">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19">
+        <v>2</v>
+      </c>
+      <c r="D1" s="19">
+        <v>3</v>
+      </c>
+      <c r="E1" s="19">
+        <v>4</v>
+      </c>
+      <c r="F1" s="19">
+        <v>5</v>
+      </c>
+      <c r="G1" s="19">
+        <v>6</v>
+      </c>
+      <c r="H1" s="19">
+        <v>7</v>
+      </c>
+      <c r="I1" s="19">
+        <v>8</v>
+      </c>
+      <c r="J1" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B2" s="13">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13">
+        <v>0</v>
+      </c>
+      <c r="J2" s="13">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="13">
+        <f ca="1">IF(RANDBETWEEN(0,3)=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="13">
+        <f t="shared" ref="C3:J10" ca="1" si="0">IF(RANDBETWEEN(0,3)=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H3" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I3" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J3" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="13">
+        <f t="shared" ref="B4:J10" ca="1" si="1">IF(RANDBETWEEN(0,3)=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I4" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="13">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C5" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="13">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C6" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D6" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" s="13">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C7" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="13">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C8" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D8" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="13">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="13">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C10" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="13">
+        <f ca="1">IF(OR(B3:B10),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="13">
+        <f t="shared" ref="C12:J12" ca="1" si="2">IF(OR(C3:C10),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="13">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="13">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H12" s="13">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="13">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="13">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="13">
+        <f ca="1">1-B12</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="13">
+        <f t="shared" ref="C13:J13" ca="1" si="3">1-C12</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="13">
+        <f ca="1">B2*B13</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="13">
+        <f t="shared" ref="C14:J14" ca="1" si="4">C2*C13</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="13">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B16" s="13">
+        <f>1-B2</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="13">
+        <f t="shared" ref="C16:J16" si="5">1-C2</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H16" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J16" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B17" s="13">
+        <f ca="1">B16+B12-B16*B12</f>
+        <v>1</v>
+      </c>
+      <c r="C17" s="13">
+        <f t="shared" ref="C17:J17" ca="1" si="6">C16+C12-C16*C12</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="13">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="13">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G17" s="13">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H17" s="13">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="13">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J17" s="13">
+        <f t="shared" ca="1" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="13">
+        <f>B16+B2-B16*B2</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="13">
+        <f t="shared" ref="C19:J19" ca="1" si="7">C16+C3-C16*C3</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="13">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G19" s="13">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H19" s="13">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="13">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="13">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="13">
+        <f ca="1">B19+B4-B19*B4</f>
+        <v>1</v>
+      </c>
+      <c r="C20" s="13">
+        <f t="shared" ref="C20:J20" ca="1" si="8">C19+C4-C19*C4</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="13">
+        <f t="shared" ca="1" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="13">
+        <f t="shared" ca="1" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G20" s="13">
+        <f t="shared" ca="1" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="H20" s="13">
+        <f t="shared" ca="1" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="I20" s="13">
+        <f t="shared" ca="1" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="13">
+        <f t="shared" ca="1" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="13">
+        <f t="shared" ref="B21:B26" ca="1" si="9">B20+B5-B20*B5</f>
+        <v>1</v>
+      </c>
+      <c r="C21" s="13">
+        <f t="shared" ref="C21:C26" ca="1" si="10">C20+C5-C20*C5</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="13">
+        <f t="shared" ref="D21:D26" ca="1" si="11">D20+D5-D20*D5</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" ref="E21:E26" si="12">E20+E5-E20*E5</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="13">
+        <f t="shared" ref="F21:F26" ca="1" si="13">F20+F5-F20*F5</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="13">
+        <f t="shared" ref="G21:G26" ca="1" si="14">G20+G5-G20*G5</f>
+        <v>1</v>
+      </c>
+      <c r="H21" s="13">
+        <f t="shared" ref="H21:H26" ca="1" si="15">H20+H5-H20*H5</f>
+        <v>1</v>
+      </c>
+      <c r="I21" s="13">
+        <f t="shared" ref="I21:I26" ca="1" si="16">I20+I5-I20*I5</f>
+        <v>1</v>
+      </c>
+      <c r="J21" s="13">
+        <f t="shared" ref="J21:J26" ca="1" si="17">J20+J5-J20*J5</f>
+        <v>1</v>
+      </c>
+      <c r="K21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="C22" s="13">
+        <f t="shared" ca="1" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D22" s="13">
+        <f t="shared" ca="1" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="13">
+        <f t="shared" ca="1" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="G22" s="13">
+        <f t="shared" ca="1" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="H22" s="13">
+        <f t="shared" ca="1" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="13">
+        <f t="shared" ca="1" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="J22" s="13">
+        <f t="shared" ca="1" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="K22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="C23" s="13">
+        <f t="shared" ca="1" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D23" s="13">
+        <f t="shared" ca="1" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="13">
+        <f t="shared" ca="1" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="G23" s="13">
+        <f t="shared" ca="1" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="13">
+        <f t="shared" ca="1" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="I23" s="13">
+        <f t="shared" ca="1" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="J23" s="13">
+        <f t="shared" ca="1" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B24" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="C24" s="13">
+        <f t="shared" ca="1" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D24" s="13">
+        <f t="shared" ca="1" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="13">
+        <f t="shared" ca="1" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="G24" s="13">
+        <f t="shared" ca="1" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="H24" s="13">
+        <f t="shared" ca="1" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="I24" s="13">
+        <f t="shared" ca="1" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="J24" s="13">
+        <f t="shared" ca="1" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="C25" s="13">
+        <f t="shared" ca="1" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D25" s="13">
+        <f t="shared" ca="1" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="13">
+        <f t="shared" ca="1" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="G25" s="13">
+        <f t="shared" ca="1" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="H25" s="13">
+        <f t="shared" ca="1" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="13">
+        <f t="shared" ca="1" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="J25" s="13">
+        <f t="shared" ca="1" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B26" s="13">
+        <f t="shared" ca="1" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="C26" s="13">
+        <f t="shared" ca="1" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D26" s="13">
+        <f t="shared" ca="1" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="13">
+        <f t="shared" ca="1" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="G26" s="13">
+        <f t="shared" ca="1" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="H26" s="13">
+        <f t="shared" ca="1" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="I26" s="13">
+        <f t="shared" ca="1" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="J26" s="13">
+        <f t="shared" ca="1" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B28" s="13">
+        <f>MOD(K28,2)</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="13">
+        <f>MOD(FLOOR(K28/2,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="13">
+        <f>MOD(FLOOR(K28/4,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="E28" s="13">
+        <f>MOD(FLOOR(K28/8,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="13">
+        <f>MOD(FLOOR(K28/16,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="G28" s="13">
+        <f>MOD(FLOOR(K28/32,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="13">
+        <f>MOD(FLOOR(K28/64,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="13">
+        <f>MOD(FLOOR(K28/128,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="13">
+        <f>MOD(FLOOR(K28/256,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>65140</v>
+      </c>
+      <c r="L28">
+        <f ca="1">K28-(256*J28+128*I28+64*H28+32*G23+16*F28+8*E28+4*D28+2*C28+B28)</f>
+        <v>65024</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="13">
+        <f>MOD(K29,2)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="13">
+        <f>MOD(FLOOR(K29/2,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="13">
+        <f>MOD(FLOOR(K29/4,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="13">
+        <f>MOD(FLOOR(K29/8,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="F29" s="13">
+        <f>MOD(FLOOR(K29/16,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="13">
+        <f>MOD(FLOOR(K29/32,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="13">
+        <f>MOD(FLOOR(K29/64,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="13">
+        <f>MOD(FLOOR(K29/128,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="13">
+        <f>MOD(FLOOR(K29/256,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B30" s="13">
+        <f>MOD(K30,2)</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="13">
+        <f>MOD(FLOOR(K30/2,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="D30" s="13">
+        <f>MOD(FLOOR(K30/4,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="13">
+        <f>MOD(FLOOR(K30/8,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="13">
+        <f>MOD(FLOOR(K30/16,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="G30" s="13">
+        <f>MOD(FLOOR(K30/32,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="H30" s="13">
+        <f>MOD(FLOOR(K30/64,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="I30" s="13">
+        <f>MOD(FLOOR(K30/128,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="13">
+        <f>MOD(FLOOR(K30/256,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>65406</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B31" s="13">
+        <f>MOD(K31,2)</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="13">
+        <f>MOD(FLOOR(K31/2,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="D31" s="13">
+        <f>MOD(FLOOR(K31/4,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="13">
+        <f>MOD(FLOOR(K31/8,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="13">
+        <f>MOD(FLOOR(K31/16,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="13">
+        <f>MOD(FLOOR(K31/32,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="13">
+        <f>MOD(FLOOR(K31/64,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="13">
+        <f>MOD(FLOOR(K31/128,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="J31" s="13">
+        <f>MOD(FLOOR(K31/256,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B32" s="13">
+        <f>MOD(K32,2)</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="13">
+        <f>MOD(FLOOR(K32/2,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="13">
+        <f>MOD(FLOOR(K32/4,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="E32" s="13">
+        <f>MOD(FLOOR(K32/8,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="F32" s="13">
+        <f>MOD(FLOOR(K32/16,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="G32" s="13">
+        <f>MOD(FLOOR(K32/32,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="H32" s="13">
+        <f>MOD(FLOOR(K32/64,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="I32" s="13">
+        <f>MOD(FLOOR(K32/128,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="J32" s="13">
+        <f>MOD(FLOOR(K32/256,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>65534</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more rules to grader (hidden pairs, hidden/naked triples, pointing pairs/triples)
</commit_message>
<xml_diff>
--- a/scratchpad/symmetry_indices.xlsx
+++ b/scratchpad/symmetry_indices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/workbench/SudokuWizard/scratchpad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E0515D-EF50-C740-9834-0D4EF7B5A940}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076560ED-D301-464D-A05D-792B9C5B447A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="460" windowWidth="13220" windowHeight="17360" activeTab="1" xr2:uid="{07FB0925-E1A7-7E43-9070-809CA48C8E41}"/>
+    <workbookView xWindow="25000" yWindow="1220" windowWidth="20380" windowHeight="17360" activeTab="1" xr2:uid="{07FB0925-E1A7-7E43-9070-809CA48C8E41}"/>
   </bookViews>
   <sheets>
     <sheet name="symmetry" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,6 +136,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -274,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -327,10 +335,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1151,10 +1162,10 @@
         <f t="shared" si="14"/>
         <v>71</v>
       </c>
-      <c r="Q8" s="18" t="s">
+      <c r="Q8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="R8" s="18"/>
+      <c r="R8" s="19"/>
       <c r="S8">
         <f t="shared" si="3"/>
         <v>71</v>
@@ -2519,10 +2530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DF1539-E103-F04B-9E2A-1C0C3B8DBAE0}">
-  <dimension ref="B1:M32"/>
+  <dimension ref="B1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2532,31 +2543,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B1" s="19">
-        <v>1</v>
-      </c>
-      <c r="C1" s="19">
+      <c r="B1" s="18">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18">
         <v>2</v>
       </c>
-      <c r="D1" s="19">
+      <c r="D1" s="18">
         <v>3</v>
       </c>
-      <c r="E1" s="19">
+      <c r="E1" s="18">
         <v>4</v>
       </c>
-      <c r="F1" s="19">
+      <c r="F1" s="18">
         <v>5</v>
       </c>
-      <c r="G1" s="19">
+      <c r="G1" s="18">
         <v>6</v>
       </c>
-      <c r="H1" s="19">
+      <c r="H1" s="18">
         <v>7</v>
       </c>
-      <c r="I1" s="19">
+      <c r="I1" s="18">
         <v>8</v>
       </c>
-      <c r="J1" s="19">
+      <c r="J1" s="18">
         <v>9</v>
       </c>
     </row>
@@ -2609,7 +2620,7 @@
       </c>
       <c r="D3" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="13">
         <v>0</v>
@@ -2628,7 +2639,7 @@
       </c>
       <c r="I3" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2643,7 +2654,7 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" s="13">
-        <f t="shared" ref="B4:J10" ca="1" si="1">IF(RANDBETWEEN(0,3)=0, 1, 0)</f>
+        <f t="shared" ref="B4:B10" ca="1" si="1">IF(RANDBETWEEN(0,3)=0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="C4" s="13">
@@ -2652,7 +2663,7 @@
       </c>
       <c r="D4" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="13">
         <v>0</v>
@@ -2667,7 +2678,7 @@
       </c>
       <c r="H4" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2675,7 +2686,7 @@
       </c>
       <c r="J4" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="s">
         <v>18</v>
@@ -2687,7 +2698,7 @@
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2714,11 +2725,11 @@
       </c>
       <c r="I5" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
@@ -2728,7 +2739,7 @@
       </c>
       <c r="C6" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2747,7 +2758,7 @@
       </c>
       <c r="H6" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2769,14 +2780,14 @@
       </c>
       <c r="D7" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="13">
         <v>0</v>
       </c>
       <c r="F7" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2788,11 +2799,11 @@
       </c>
       <c r="I7" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
@@ -2802,11 +2813,11 @@
       </c>
       <c r="C8" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="13">
         <v>0</v>
@@ -2825,7 +2836,7 @@
       </c>
       <c r="I8" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2854,7 +2865,7 @@
       </c>
       <c r="G9" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2862,7 +2873,7 @@
       </c>
       <c r="I9" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2872,7 +2883,7 @@
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2887,7 +2898,7 @@
       </c>
       <c r="F10" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2899,7 +2910,7 @@
       </c>
       <c r="I10" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="13">
         <f t="shared" ca="1" si="0"/>
@@ -2913,7 +2924,7 @@
       </c>
       <c r="C12" s="13">
         <f t="shared" ref="C12:J12" ca="1" si="2">IF(OR(C3:C10),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="13">
         <f t="shared" ca="1" si="2"/>
@@ -2954,7 +2965,7 @@
       </c>
       <c r="C13" s="13">
         <f t="shared" ref="C13:J13" ca="1" si="3">1-C12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="13">
         <f t="shared" ca="1" si="3"/>
@@ -2995,7 +3006,7 @@
       </c>
       <c r="C14" s="13">
         <f t="shared" ref="C14:J14" ca="1" si="4">C2*C13</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="13">
         <f t="shared" ca="1" si="4"/>
@@ -3077,7 +3088,7 @@
       </c>
       <c r="C17" s="13">
         <f t="shared" ref="C17:J17" ca="1" si="6">C16+C12-C16*C12</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="13">
         <f t="shared" ca="1" si="6"/>
@@ -3241,7 +3252,7 @@
       </c>
       <c r="C22" s="13">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="13">
         <f t="shared" ca="1" si="11"/>
@@ -3282,7 +3293,7 @@
       </c>
       <c r="C23" s="13">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="13">
         <f t="shared" ca="1" si="11"/>
@@ -3323,7 +3334,7 @@
       </c>
       <c r="C24" s="13">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="13">
         <f t="shared" ca="1" si="11"/>
@@ -3364,7 +3375,7 @@
       </c>
       <c r="C25" s="13">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="13">
         <f t="shared" ca="1" si="11"/>
@@ -3405,7 +3416,7 @@
       </c>
       <c r="C26" s="13">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="13">
         <f t="shared" ca="1" si="11"/>
@@ -3442,15 +3453,15 @@
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28" s="13">
         <f>MOD(K28,2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="13">
         <f>MOD(FLOOR(K28/2,1),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="13">
         <f>MOD(FLOOR(K28/4,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="13">
         <f>MOD(FLOOR(K28/8,1),2)</f>
@@ -3458,11 +3469,11 @@
       </c>
       <c r="F28" s="13">
         <f>MOD(FLOOR(K28/16,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" s="13">
         <f>MOD(FLOOR(K28/32,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="13">
         <f>MOD(FLOOR(K28/64,1),2)</f>
@@ -3474,14 +3485,14 @@
       </c>
       <c r="J28" s="13">
         <f>MOD(FLOOR(K28/256,1),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28">
-        <v>65140</v>
+        <v>323</v>
       </c>
       <c r="L28">
         <f ca="1">K28-(256*J28+128*I28+64*H28+32*G23+16*F28+8*E28+4*D28+2*C28+B28)</f>
-        <v>65024</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
@@ -3491,15 +3502,15 @@
       </c>
       <c r="C29" s="13">
         <f>MOD(FLOOR(K29/2,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="13">
         <f>MOD(FLOOR(K29/4,1),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="13">
         <f>MOD(FLOOR(K29/8,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="13">
         <f>MOD(FLOOR(K29/16,1),2)</f>
@@ -3507,11 +3518,11 @@
       </c>
       <c r="G29" s="13">
         <f>MOD(FLOOR(K29/32,1),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="13">
         <f>MOD(FLOOR(K29/64,1),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="13">
         <f>MOD(FLOOR(K29/128,1),2)</f>
@@ -3522,13 +3533,13 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <v>266</v>
+        <v>356</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" s="13">
         <f>MOD(K30,2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="13">
         <f>MOD(FLOOR(K30/2,1),2)</f>
@@ -3540,11 +3551,11 @@
       </c>
       <c r="E30" s="13">
         <f>MOD(FLOOR(K30/8,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" s="13">
         <f>MOD(FLOOR(K30/16,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" s="13">
         <f>MOD(FLOOR(K30/32,1),2)</f>
@@ -3563,17 +3574,17 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <v>65406</v>
+        <v>359</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31" s="13">
         <f>MOD(K31,2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="13">
         <f>MOD(FLOOR(K31/2,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="13">
         <f>MOD(FLOOR(K31/4,1),2)</f>
@@ -3581,7 +3592,7 @@
       </c>
       <c r="E31" s="13">
         <f>MOD(FLOOR(K31/8,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="13">
         <f>MOD(FLOOR(K31/16,1),2)</f>
@@ -3589,22 +3600,22 @@
       </c>
       <c r="G31" s="13">
         <f>MOD(FLOOR(K31/32,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="13">
         <f>MOD(FLOOR(K31/64,1),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="13">
         <f>MOD(FLOOR(K31/128,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" s="13">
         <f>MOD(FLOOR(K31/256,1),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31">
-        <v>170</v>
+        <v>321</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
@@ -3622,11 +3633,11 @@
       </c>
       <c r="E32" s="13">
         <f>MOD(FLOOR(K32/8,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" s="13">
         <f>MOD(FLOOR(K32/16,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="13">
         <f>MOD(FLOOR(K32/32,1),2)</f>
@@ -3634,18 +3645,249 @@
       </c>
       <c r="H32" s="13">
         <f>MOD(FLOOR(K32/64,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" s="13">
         <f>MOD(FLOOR(K32/128,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" s="13">
         <f>MOD(FLOOR(K32/256,1),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32">
-        <v>65534</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="13">
+        <f t="shared" ref="B33:B35" si="18">MOD(K33,2)</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="13">
+        <f t="shared" ref="C33:C35" si="19">MOD(FLOOR(K33/2,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="13">
+        <f t="shared" ref="D33:D35" si="20">MOD(FLOOR(K33/4,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="E33" s="13">
+        <f t="shared" ref="E33:E35" si="21">MOD(FLOOR(K33/8,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="13">
+        <f t="shared" ref="F33:F35" si="22">MOD(FLOOR(K33/16,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="13">
+        <f t="shared" ref="G33:G35" si="23">MOD(FLOOR(K33/32,1),2)</f>
+        <v>1</v>
+      </c>
+      <c r="H33" s="13">
+        <f t="shared" ref="H33:H35" si="24">MOD(FLOOR(K33/64,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="13">
+        <f t="shared" ref="I33:I35" si="25">MOD(FLOOR(K33/128,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="13">
+        <f t="shared" ref="J33:J35" si="26">MOD(FLOOR(K33/256,1),2)</f>
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" s="13">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="C34" s="13">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="D34" s="13">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="E34" s="13">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="13">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="13">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="H34" s="13">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="13">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="13">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35" s="13">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="C35" s="13">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="D35" s="13">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="13">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="13">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="13">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="H35" s="13">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="13">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="13">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B37" s="13">
+        <v>0</v>
+      </c>
+      <c r="C37" s="13">
+        <v>1</v>
+      </c>
+      <c r="D37" s="13">
+        <v>0</v>
+      </c>
+      <c r="E37" s="13">
+        <v>0</v>
+      </c>
+      <c r="F37" s="13">
+        <v>0</v>
+      </c>
+      <c r="G37" s="13">
+        <v>1</v>
+      </c>
+      <c r="H37" s="13">
+        <v>0</v>
+      </c>
+      <c r="I37" s="13">
+        <v>0</v>
+      </c>
+      <c r="J37" s="13">
+        <v>0</v>
+      </c>
+      <c r="K37" s="13">
+        <f>SUM(B39:J39)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B38" s="20">
+        <v>1</v>
+      </c>
+      <c r="C38" s="20">
+        <f>B38*2</f>
+        <v>2</v>
+      </c>
+      <c r="D38" s="20">
+        <f t="shared" ref="D38:J38" si="27">C38*2</f>
+        <v>4</v>
+      </c>
+      <c r="E38" s="20">
+        <f t="shared" si="27"/>
+        <v>8</v>
+      </c>
+      <c r="F38" s="20">
+        <f t="shared" si="27"/>
+        <v>16</v>
+      </c>
+      <c r="G38" s="20">
+        <f t="shared" si="27"/>
+        <v>32</v>
+      </c>
+      <c r="H38" s="20">
+        <f t="shared" si="27"/>
+        <v>64</v>
+      </c>
+      <c r="I38" s="20">
+        <f t="shared" si="27"/>
+        <v>128</v>
+      </c>
+      <c r="J38" s="20">
+        <f t="shared" si="27"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B39" s="20">
+        <f>B37*B38</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="20">
+        <f t="shared" ref="C39:J39" si="28">C37*C38</f>
+        <v>2</v>
+      </c>
+      <c r="D39" s="20">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="20">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="20">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="G39" s="20">
+        <f t="shared" si="28"/>
+        <v>32</v>
+      </c>
+      <c r="H39" s="20">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="20">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="20">
+        <f t="shared" si="28"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>